<commit_message>
Update notebooks with 2023 data
And create new figures
</commit_message>
<xml_diff>
--- a/data/update_2023/Publications_Scopus_WoS_2003_2023.xlsx
+++ b/data/update_2023/Publications_Scopus_WoS_2003_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smasneri\CODE\AR_SLR_Paper\data\update_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0F7F603-00F7-4419-A57C-9EE6932D5613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65E32FE-B129-4BDC-95C5-68E431276A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="675" windowWidth="27975" windowHeight="14550" xr2:uid="{B4ECF6A1-03F6-494F-8D8C-EAFE412ECD8A}"/>
+    <workbookView xWindow="29340" yWindow="795" windowWidth="27975" windowHeight="14550" xr2:uid="{B4ECF6A1-03F6-494F-8D8C-EAFE412ECD8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Your query : (TITLE-ABS-KEY("Augmented Reality" AND "Education"))</t>
-  </si>
-  <si>
-    <t>Year range: 2003-2023</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>SCOPUS</t>
   </si>
   <si>
     <t>WOS</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -399,260 +396,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AA98D3-77CE-4E8B-8846-E16DCCD6AC6D}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>2003</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2004</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="A4">
+        <v>2005</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="B9">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C9">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2008</v>
+        <v>2011</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="C10">
-        <v>42</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="B11">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="C11">
-        <v>51</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>185</v>
       </c>
       <c r="C12">
-        <v>76</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="B13">
-        <v>104</v>
+        <v>190</v>
       </c>
       <c r="C13">
-        <v>119</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="B14">
-        <v>124</v>
+        <v>290</v>
       </c>
       <c r="C14">
-        <v>138</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="B15">
-        <v>185</v>
+        <v>276</v>
       </c>
       <c r="C15">
-        <v>217</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="B16">
-        <v>190</v>
+        <v>469</v>
       </c>
       <c r="C16">
-        <v>211</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B17">
-        <v>290</v>
+        <v>572</v>
       </c>
       <c r="C17">
-        <v>273</v>
+        <v>659</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B18">
-        <v>276</v>
+        <v>773</v>
       </c>
       <c r="C18">
-        <v>315</v>
+        <v>934</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="B19">
-        <v>469</v>
+        <v>866</v>
       </c>
       <c r="C19">
-        <v>469</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B20">
-        <v>572</v>
+        <v>982</v>
       </c>
       <c r="C20">
-        <v>659</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="B21">
-        <v>773</v>
+        <v>1102</v>
       </c>
       <c r="C21">
-        <v>934</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="B22">
-        <v>866</v>
+        <v>1017</v>
       </c>
       <c r="C22">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2021</v>
-      </c>
-      <c r="B23">
-        <v>982</v>
-      </c>
-      <c r="C23">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2022</v>
-      </c>
-      <c r="B24">
-        <v>1102</v>
-      </c>
-      <c r="C24">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2023</v>
-      </c>
-      <c r="B25">
-        <v>1017</v>
-      </c>
-      <c r="C25">
         <v>874</v>
       </c>
     </row>

</xml_diff>